<commit_message>
Updated cross-walk between WDFW and NWFSC survey sites; created data file for sea otter counts (only entered 1977-2004 so far)
</commit_message>
<xml_diff>
--- a/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
+++ b/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="460" windowWidth="41620" windowHeight="20900" tabRatio="500"/>
+    <workbookView xWindow="12020" yWindow="1060" windowWidth="41620" windowHeight="20900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
   <si>
     <t>Neah Bay</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Cape Johnson/Bluff Point</t>
   </si>
   <si>
-    <t>Carrol Island/ Sea Lion Rock Sandy Island</t>
-  </si>
-  <si>
     <t>Perkins Reef (Rock 443)</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t xml:space="preserve">Point Of Arches </t>
   </si>
   <si>
-    <t>West End Of Bodelteh Islands Duk Point</t>
-  </si>
-  <si>
     <t>Father And Son</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>https://www.nps.gov/olym/planyourvisit/upload/OLYMmap1.pdf</t>
   </si>
   <si>
-    <t>Southeast of Ozette Island, Ozette/Cape Alava/Bodelteh Islands, West End Of Bodelteh Islands Duk Point</t>
-  </si>
-  <si>
     <t xml:space="preserve">Father And Son, Point Of Arches </t>
   </si>
   <si>
@@ -207,13 +198,136 @@
   </si>
   <si>
     <t>Anderson Pt., Anderson Pt. (Osprey I), Makah Bay</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>Site code for analysis</t>
+  </si>
+  <si>
+    <t>Makah Bay/Waatch Pt.</t>
+  </si>
+  <si>
+    <t>Portage Head/Anderson Pt</t>
+  </si>
+  <si>
+    <t>Anderson Point, Makah Bay/Waatch Pt., Portage Head/Anderson Pt</t>
+  </si>
+  <si>
+    <t>Duk Point</t>
+  </si>
+  <si>
+    <t>West End Of Bodelteh Islands</t>
+  </si>
+  <si>
+    <t>Ozette River</t>
+  </si>
+  <si>
+    <t>W Bodelteh</t>
+  </si>
+  <si>
+    <t>Ozette/Cape Alava</t>
+  </si>
+  <si>
+    <t>S.Ozette Island</t>
+  </si>
+  <si>
+    <t>Ozette/Cape Alava/Bodelteh Islands, West End Of Bodelteh Islands, W Bodelteh, Ozette/Cape Alava</t>
+  </si>
+  <si>
+    <t>White Rock</t>
+  </si>
+  <si>
+    <t>Submarine Rock</t>
+  </si>
+  <si>
+    <t>North Point</t>
+  </si>
+  <si>
+    <t>Yellow B Area</t>
+  </si>
+  <si>
+    <t>Off Yellow B</t>
+  </si>
+  <si>
+    <t>Cedar Creek</t>
+  </si>
+  <si>
+    <t>Carroll Island</t>
+  </si>
+  <si>
+    <t>Carrol Island/ Sea Lion Rock</t>
+  </si>
+  <si>
+    <t>Sandy Island</t>
+  </si>
+  <si>
+    <t>Bluff Point</t>
+  </si>
+  <si>
+    <t>South of Cape Johnson/Chilean Memorial, Cape Johnson, S. Cape Johnson</t>
+  </si>
+  <si>
+    <t>S. Cape Johnson</t>
+  </si>
+  <si>
+    <t>CJR3</t>
+  </si>
+  <si>
+    <t>James Island</t>
+  </si>
+  <si>
+    <t>Quillayute Needles</t>
+  </si>
+  <si>
+    <t>Giants Graveyard</t>
+  </si>
+  <si>
+    <t>Giants Graveyard/Teahwhit Head, Giants Graveyard</t>
+  </si>
+  <si>
+    <t>Toleak/Strawberry</t>
+  </si>
+  <si>
+    <t>Hoh R/Perkins R</t>
+  </si>
+  <si>
+    <t>Destruction Is.</t>
+  </si>
+  <si>
+    <t>Destruction Island, Destruction Is.</t>
+  </si>
+  <si>
+    <t>Willoughby Rk.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,6 +374,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -295,7 +416,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -306,6 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -585,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,24 +721,27 @@
     <col min="6" max="6" width="86.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -624,33 +749,39 @@
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -658,33 +789,39 @@
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -695,13 +832,16 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,16 +849,19 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -726,16 +869,19 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -751,16 +897,19 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>0</v>
@@ -768,8 +917,11 @@
       <c r="G10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,47 +935,50 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -831,41 +986,41 @@
         <v>9</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
-        <v>30</v>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>35</v>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>36</v>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -875,42 +1030,165 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C24" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="7" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="7" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C29" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C30" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added site codes to all data, updated lookup tables
</commit_message>
<xml_diff>
--- a/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
+++ b/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameal.samhouri/Documents/Github/OCNMS/Data/Xls files and READMEs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12020" yWindow="1060" windowWidth="41620" windowHeight="20900" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
   <si>
     <t>Neah Bay</t>
   </si>
@@ -185,9 +180,6 @@
     <t>https://www.nps.gov/olym/planyourvisit/upload/OLYMmap1.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Father And Son, Point Of Arches </t>
-  </si>
-  <si>
     <t>Shipwreck Point</t>
   </si>
   <si>
@@ -233,9 +225,6 @@
     <t>Portage Head/Anderson Pt</t>
   </si>
   <si>
-    <t>Anderson Point, Makah Bay/Waatch Pt., Portage Head/Anderson Pt</t>
-  </si>
-  <si>
     <t>Duk Point</t>
   </si>
   <si>
@@ -254,9 +243,6 @@
     <t>S.Ozette Island</t>
   </si>
   <si>
-    <t>Ozette/Cape Alava/Bodelteh Islands, West End Of Bodelteh Islands, W Bodelteh, Ozette/Cape Alava</t>
-  </si>
-  <si>
     <t>White Rock</t>
   </si>
   <si>
@@ -287,9 +273,6 @@
     <t>Bluff Point</t>
   </si>
   <si>
-    <t>South of Cape Johnson/Chilean Memorial, Cape Johnson, S. Cape Johnson</t>
-  </si>
-  <si>
     <t>S. Cape Johnson</t>
   </si>
   <si>
@@ -317,10 +300,166 @@
     <t>Destruction Is.</t>
   </si>
   <si>
-    <t>Destruction Island, Destruction Is.</t>
-  </si>
-  <si>
     <t>Willoughby Rk.</t>
+  </si>
+  <si>
+    <t>Offshore Yellow Banks</t>
+  </si>
+  <si>
+    <t>1 MILE W. OF HOH HEAD (IN OPEN WATER)</t>
+  </si>
+  <si>
+    <t>Alexander Island</t>
+  </si>
+  <si>
+    <t>Bahobohosh Point</t>
+  </si>
+  <si>
+    <t>Browns Point</t>
+  </si>
+  <si>
+    <t>Chilean Memorial</t>
+  </si>
+  <si>
+    <t>DESTRUCTION ISLAND WEST END</t>
+  </si>
+  <si>
+    <t>DESTRUCTION I.  EAST END</t>
+  </si>
+  <si>
+    <t>Destruction Island, Destruction Is., DESTRUCTION I.  EAST END, DESTRUCTION ISLAND WEST END</t>
+  </si>
+  <si>
+    <t>Fuca Pillar</t>
+  </si>
+  <si>
+    <t>Hogsback</t>
+  </si>
+  <si>
+    <t>Hoh Head</t>
+  </si>
+  <si>
+    <t>HOH RIVER MOUTH</t>
+  </si>
+  <si>
+    <t>INSHORE KELP BED EAST OF WHITE ROCK</t>
+  </si>
+  <si>
+    <t>INSHORE OF FATHER AND SON</t>
+  </si>
+  <si>
+    <t>Father And Son, Point Of Arches, INSHORE OF FATHER AND SON</t>
+  </si>
+  <si>
+    <t>INSHORE WHITE ROCK</t>
+  </si>
+  <si>
+    <t>MIDDLE Rk/DIAMOND ROCK</t>
+  </si>
+  <si>
+    <t>MIDWAY BEACH</t>
+  </si>
+  <si>
+    <t>MIDWAY POINT</t>
+  </si>
+  <si>
+    <t>Mushroom Rock</t>
+  </si>
+  <si>
+    <t>N. OF ANDERSON POINT</t>
+  </si>
+  <si>
+    <t>N. OF CAPE JOHNSON</t>
+  </si>
+  <si>
+    <t>N. OF HOH HEAD</t>
+  </si>
+  <si>
+    <t>NORTH BROWN PT.</t>
+  </si>
+  <si>
+    <t>NORTH KAYOSTLA BEACH</t>
+  </si>
+  <si>
+    <t>NORTH ROCK</t>
+  </si>
+  <si>
+    <t>NORTH STEAMBOAT CREEK</t>
+  </si>
+  <si>
+    <t>OZETTE I.</t>
+  </si>
+  <si>
+    <t>OZETTE ISLAND</t>
+  </si>
+  <si>
+    <t>Rialto Beach</t>
+  </si>
+  <si>
+    <t>ROCK 443 COMPLEX</t>
+  </si>
+  <si>
+    <t>RUBY BEACH</t>
+  </si>
+  <si>
+    <t>S. CAPE JOHNSON/CHILEAN MEMORIAL</t>
+  </si>
+  <si>
+    <t>S. OF CHILEAN MEMORIAL</t>
+  </si>
+  <si>
+    <t>South of Cape Johnson/Chilean Memorial, Cape Johnson, S. Cape Johnson, CAPE JOHNSON/BLUFF POINT, Chilean Memorial, N. OF CAPE JOHNSON, S. CAPE JOHNSON/CHILEAN MEMORIAL, S. OF CHILEAN MEMORIAL</t>
+  </si>
+  <si>
+    <t>S. OF OZETTE RIVER</t>
+  </si>
+  <si>
+    <t>S. PORTAGE HEAD</t>
+  </si>
+  <si>
+    <t>SANDY ISLET/JAGGED ISLAND AREA</t>
+  </si>
+  <si>
+    <t>http://www.alertdiver.com/Washingtons_Olympic_Peninsula</t>
+  </si>
+  <si>
+    <t>Slant Rock</t>
+  </si>
+  <si>
+    <t>Tatoosh Island, Mushroom Rock, Slant Rock</t>
+  </si>
+  <si>
+    <t>SOUTH END OZETTE ISLAND</t>
+  </si>
+  <si>
+    <t>SOUTH OF OZETTE RIVER</t>
+  </si>
+  <si>
+    <t>SOUTH OF PORTAGE HEAD</t>
+  </si>
+  <si>
+    <t>SOUTH RAFT RIVER</t>
+  </si>
+  <si>
+    <t>UMATILLA REEF</t>
+  </si>
+  <si>
+    <t>Waddah Island</t>
+  </si>
+  <si>
+    <t>WAATCH PT.</t>
+  </si>
+  <si>
+    <t>Anderson Point, Makah Bay/Waatch Pt., Portage Head/Anderson Pt, Bahobohosh Point, MAKAH BAY, N. OF ANDERSON POINT, S. PORTAGE HEAD, SOUTH OF PORTAGE HEAD, WAATCH PT.</t>
+  </si>
+  <si>
+    <t>WEDDING ROCKS</t>
+  </si>
+  <si>
+    <t>Ozette/Cape Alava/Bodelteh Islands, West End Of Bodelteh Islands, W Bodelteh, Ozette/Cape Alava, OZETTE I., OZETTE ISLAND, Ozette River, S.Ozette Island, Southeast of Ozette Island, S. OF OZETTE RIVER, SOUTH END OZETTE ISLAND, SOUTH OF OZETTE RIVER, UMATILLA REEF, WEST END OF BODELTEH</t>
+  </si>
+  <si>
+    <t>WEST END OF BODELTEH</t>
   </si>
 </sst>
 </file>
@@ -411,8 +550,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -429,9 +624,65 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,7 +738,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -522,7 +773,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -699,7 +950,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -707,13 +958,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
@@ -721,7 +972,7 @@
     <col min="6" max="6" width="86.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
@@ -738,175 +989,175 @@
         <v>48</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>49</v>
+      <c r="C3" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>20</v>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
+      <c r="C6" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
+      <c r="C8" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>24</v>
+      <c r="C9" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
@@ -918,15 +1169,15 @@
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
+      <c r="C11" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>0</v>
@@ -935,266 +1186,515 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3">
+      <c r="C79" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="6" t="s">
+    <row r="83" spans="3:3">
+      <c r="C83" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C29" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="5" t="s">
+    <row r="95" spans="3:3">
+      <c r="C95" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3">
+      <c r="C97" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3">
+      <c r="C99" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3">
+      <c r="C100" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3">
+      <c r="C101" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="5" t="s">
+    <row r="102" spans="3:3">
+      <c r="C102" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C45" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C46" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C48" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55" s="5" t="s">
-        <v>97</v>
+    <row r="103" spans="3:3">
+      <c r="C103" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A19">
-    <sortCondition ref="A1:A19"/>
+  <sortState ref="C2:C55">
+    <sortCondition ref="C2:C55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed cross check of 2000-2004 sea otter data. All site and region codes are correct too. Ready for plotting.
</commit_message>
<xml_diff>
--- a/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
+++ b/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="147">
   <si>
     <t>Neah Bay</t>
   </si>
@@ -408,9 +408,6 @@
     <t>S. OF CHILEAN MEMORIAL</t>
   </si>
   <si>
-    <t>South of Cape Johnson/Chilean Memorial, Cape Johnson, S. Cape Johnson, CAPE JOHNSON/BLUFF POINT, Chilean Memorial, N. OF CAPE JOHNSON, S. CAPE JOHNSON/CHILEAN MEMORIAL, S. OF CHILEAN MEMORIAL</t>
-  </si>
-  <si>
     <t>S. OF OZETTE RIVER</t>
   </si>
   <si>
@@ -450,9 +447,6 @@
     <t>WAATCH PT.</t>
   </si>
   <si>
-    <t>Anderson Point, Makah Bay/Waatch Pt., Portage Head/Anderson Pt, Bahobohosh Point, MAKAH BAY, N. OF ANDERSON POINT, S. PORTAGE HEAD, SOUTH OF PORTAGE HEAD, WAATCH PT.</t>
-  </si>
-  <si>
     <t>WEDDING ROCKS</t>
   </si>
   <si>
@@ -460,6 +454,15 @@
   </si>
   <si>
     <t>WEST END OF BODELTEH</t>
+  </si>
+  <si>
+    <t>Shi Shi Beach</t>
+  </si>
+  <si>
+    <t>Anderson Point, Makah Bay/Waatch Pt., Portage Head/Anderson Pt, Bahobohosh Point, MAKAH BAY, N. OF ANDERSON POINT, S. PORTAGE HEAD, SOUTH OF PORTAGE HEAD, WAATCH PT., Shi Shi Beach</t>
+  </si>
+  <si>
+    <t>South of Cape Johnson/Chilean Memorial, Cape Johnson, S. Cape Johnson, CAPE JOHNSON/BLUFF POINT, Chilean Memorial, N. OF CAPE JOHNSON, S. CAPE JOHNSON/CHILEAN MEMORIAL, S. OF CHILEAN MEMORIAL, BLUFF POINT</t>
   </si>
 </sst>
 </file>
@@ -550,8 +553,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -624,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -654,6 +661,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -683,6 +692,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1043,7 +1054,7 @@
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
@@ -1063,7 +1074,7 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
@@ -1083,7 +1094,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>4</v>
@@ -1096,7 +1107,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1123,7 +1134,7 @@
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G8" t="s">
         <v>55</v>
@@ -1143,7 +1154,7 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
@@ -1251,7 +1262,7 @@
         <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1532,12 +1543,12 @@
     </row>
     <row r="73" spans="3:3">
       <c r="C73" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="3:3">
@@ -1552,7 +1563,7 @@
     </row>
     <row r="77" spans="3:3">
       <c r="C77" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="3:3">
@@ -1562,126 +1573,131 @@
     </row>
     <row r="79" spans="3:3">
       <c r="C79" s="6" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" s="6" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="6" t="s">
-        <v>127</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="6" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="6" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="3:3">
-      <c r="C86" s="5" t="s">
-        <v>138</v>
+      <c r="C86" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="3:3">
-      <c r="C88" s="6" t="s">
+    <row r="89" spans="3:3">
+      <c r="C89" s="6" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="3:3">
-      <c r="C89" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="91" spans="3:3">
-      <c r="C91" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96" s="5" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3">
-      <c r="C93" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3">
-      <c r="C94" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3">
-      <c r="C95" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3">
-      <c r="C96" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="6" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3">
-      <c r="C98" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="5" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="5" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="5" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="5" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated sea otter site assignments
</commit_message>
<xml_diff>
--- a/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
+++ b/Data/Xls files and READMEs/Study sites Kvitek WDFW NWFSC.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Site assignments June 2017" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="158">
   <si>
     <t>Neah Bay</t>
   </si>
@@ -463,6 +464,39 @@
   </si>
   <si>
     <t>South of Cape Johnson/Chilean Memorial, Cape Johnson, S. Cape Johnson, CAPE JOHNSON/BLUFF POINT, Chilean Memorial, N. OF CAPE JOHNSON, S. CAPE JOHNSON/CHILEAN MEMORIAL, S. OF CHILEAN MEMORIAL, BLUFF POINT</t>
+  </si>
+  <si>
+    <t>Regional borders for summing otter counts</t>
+  </si>
+  <si>
+    <t>Quillayute River mouth (La Push) south to Toleak Point</t>
+  </si>
+  <si>
+    <t>Norwegian Memorial south to Quillayute River mouth (La Push); same as Rock 305</t>
+  </si>
+  <si>
+    <t>Norwegian Memorial south to Quillayute River mouth (La Push); same as Cape Johnson</t>
+  </si>
+  <si>
+    <t>Ozette River mouth south to Norwegian Memorial</t>
+  </si>
+  <si>
+    <t>North end of Shi Shi Beach south to Ozette River mouth</t>
+  </si>
+  <si>
+    <t>Cape Flattery South to north end of Shi Shi Beach</t>
+  </si>
+  <si>
+    <t>Cape Flattery north and east to Chibadehl Rocks; same as Chibadehl Rocks</t>
+  </si>
+  <si>
+    <t>Cape Flattery north and east to Chibadehl Rocks; same as Tatoosh Island</t>
+  </si>
+  <si>
+    <t>Chibadehl Rocks east to Neah Bay</t>
+  </si>
+  <si>
+    <t>Toleak Point south to Point Grenville</t>
   </si>
 </sst>
 </file>
@@ -553,8 +587,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -631,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -663,6 +711,13 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -694,6 +749,13 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -961,7 +1023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -969,10 +1031,789 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="86.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3">
+      <c r="C79" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3">
+      <c r="C97" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3">
+      <c r="C99" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3">
+      <c r="C100" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3">
+      <c r="C101" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3">
+      <c r="C102" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3">
+      <c r="C103" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>